<commit_message>
Incorporation of github repo link
</commit_message>
<xml_diff>
--- a/MT-Python-Programming/MT-Python-Lectures.xlsx
+++ b/MT-Python-Programming/MT-Python-Lectures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ramrustagi/OneDrive - Advanced Computing and Communications Society/Academic/Presentations/RPR-2019-20/MT-Programming-with-Python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FF90401-D01F-5A4D-9BC7-7552A9F6C0FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BB6A20D-3403-AA48-9F9E-886E6E477EEA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="960" windowWidth="16140" windowHeight="14680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>2020-MT-L01-Intro-Programming.pdf</t>
   </si>
@@ -136,6 +136,30 @@
   </si>
   <si>
     <t>https://youtu.be/Vg1mve_o97M</t>
+  </si>
+  <si>
+    <t>Data Visualization</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=Z8b90hUig_s</t>
+  </si>
+  <si>
+    <t>Multi graph plotting</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=ZtxB8DS1NEE</t>
+  </si>
+  <si>
+    <t>2020-MT-L12-Visualization.pdf</t>
+  </si>
+  <si>
+    <t>2020-MT-L13-MultiPlots.pdf</t>
+  </si>
+  <si>
+    <t>GitHub link for all lectures</t>
+  </si>
+  <si>
+    <t>https://github.com/rprustagi/EL-Programming-with-Python.git</t>
   </si>
 </sst>
 </file>
@@ -976,10 +1000,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -991,201 +1015,215 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>10</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
         <v>11</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C2" t="s">
         <v>12</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D2" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" t="s">
-        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
-        <f>A2+1</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" t="s">
-        <v>33</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
-        <f t="shared" ref="A4:A16" si="0">A3+1</f>
-        <v>3</v>
+        <f>A3+1</f>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5">
-        <f t="shared" si="0"/>
-        <v>4</v>
+        <f t="shared" ref="A5:A15" si="0">A4+1</f>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D7" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D9" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D10" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D11" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C12" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="D12" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15">
         <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <f t="shared" si="0"/>
-        <v>15</v>
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>